<commit_message>
Add disclaimer to example data set
</commit_message>
<xml_diff>
--- a/example-data.xlsx
+++ b/example-data.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t xml:space="preserve">Software Version</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t xml:space="preserve">Experiment File Path:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">THIS IS JUST AN EXAMPLE</t>
   </si>
   <si>
     <t xml:space="preserve">Protocol File Path:</t>
@@ -534,10 +537,10 @@
   <dimension ref="A2:O42"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.60546875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.61328125" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.78"/>
@@ -551,27 +554,30 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="B4" s="0" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>43333</v>
@@ -579,7 +585,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8" s="2" t="n">
         <v>0.599699074074074</v>
@@ -587,15 +593,15 @@
     </row>
     <row r="9" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>111111</v>
@@ -603,71 +609,71 @@
     </row>
     <row r="11" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B13" s="4"/>
     </row>
     <row r="14" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B22" s="4"/>
     </row>
     <row r="23" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>24.2</v>
@@ -675,7 +681,7 @@
     </row>
     <row r="24" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>24.2</v>
@@ -722,7 +728,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B27" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C27" s="7" t="n">
         <v>1.731</v>
@@ -808,7 +814,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B29" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C29" s="18" t="n">
         <v>1.333</v>
@@ -894,7 +900,7 @@
     </row>
     <row r="31" customFormat="false" ht="13.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B31" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C31" s="19" t="n">
         <v>0.902</v>
@@ -980,7 +986,7 @@
     </row>
     <row r="33" customFormat="false" ht="13.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B33" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C33" s="11" t="n">
         <v>0.723</v>
@@ -1066,7 +1072,7 @@
     </row>
     <row r="35" customFormat="false" ht="13.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B35" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C35" s="13" t="n">
         <v>0.295</v>
@@ -1152,7 +1158,7 @@
     </row>
     <row r="37" customFormat="false" ht="13.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B37" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C37" s="8" t="n">
         <v>0.164</v>
@@ -1238,7 +1244,7 @@
     </row>
     <row r="39" customFormat="false" ht="13.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B39" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C39" s="25" t="n">
         <v>0.096</v>
@@ -1324,7 +1330,7 @@
     </row>
     <row r="41" customFormat="false" ht="13.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B41" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C41" s="25" t="n">
         <v>0.07</v>

</xml_diff>